<commit_message>
Termine el primer requerimientoooooo :)
</commit_message>
<xml_diff>
--- a/CarDealer/docs/traceabillity.xlsx
+++ b/CarDealer/docs/traceabillity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo Ramos\Desktop\Lab3\CarDealer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24BA7029-3776-457B-B837-C397BE3A3587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E738054C-CA6B-4042-9F03-DEE535682D9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
+    <workbookView xWindow="4344" yWindow="-60" windowWidth="17280" windowHeight="8964" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Requirements</t>
   </si>
@@ -72,9 +72,6 @@
     <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double) : String</t>
   </si>
   <si>
-    <t>registerVehicle(price : double, brand : String, model : int, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double, batteryConsume : double) : String</t>
-  </si>
-  <si>
     <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double, typeCharger : int, batteryDuration : double, batteryConsume : double) : String</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
     <t>GasolineCar(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double)</t>
   </si>
   <si>
-    <t>ElectricCar(price : double, brand : String, model : int, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double, batteryConsume : double)</t>
-  </si>
-  <si>
     <t>HybridCar(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double, typeCharger : int, batteryDuration : double, batteryConsume : double)</t>
   </si>
   <si>
@@ -124,6 +118,18 @@
   </si>
   <si>
     <t>getLicensePlate() : String</t>
+  </si>
+  <si>
+    <t>ElectricCar(price : double, brand : String, model : int,displacement:double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double, batteryConsume : double)</t>
+  </si>
+  <si>
+    <t>registerVehicle(price : double, brand : String, model : int, displacement:double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double, batteryConsume : double) : String</t>
+  </si>
+  <si>
+    <t>saveInParkingLot(model : int, isNew : boolean) : boolean</t>
+  </si>
+  <si>
+    <t>lookForSpaceinParkingLot(column : int) : int</t>
   </si>
 </sst>
 </file>
@@ -177,11 +183,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -189,15 +192,21 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -513,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE54D6B-CD4A-424B-9A43-965713A2DE34}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="69" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -527,37 +536,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6" t="s">
+      <c r="A3" s="9"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5"/>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="9"/>
+      <c r="B4" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
@@ -565,129 +574,140 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5"/>
-      <c r="B5" s="1"/>
+      <c r="A5" s="9"/>
+      <c r="B5" s="8"/>
       <c r="C5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="3" t="s">
+      <c r="A6" s="9"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="3" t="s">
+      <c r="A7" s="9"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="5"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="3" t="s">
+      <c r="A8" s="9"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="5"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="3" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="8"/>
+      <c r="C11" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="5"/>
-      <c r="B11" s="1"/>
-      <c r="C11" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="8"/>
+      <c r="C12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="5"/>
-      <c r="B12" s="1"/>
-      <c r="C12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="8"/>
+      <c r="C14" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="5"/>
-      <c r="B13" s="7" t="s">
+      <c r="C15" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="9"/>
+      <c r="B16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="5"/>
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" t="s">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="5"/>
-      <c r="B15" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="8" t="s">
+    </row>
+    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="5"/>
-      <c r="B16" s="2" t="s">
+      <c r="C18" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C19" s="6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A17" s="5"/>
-      <c r="B17" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="8" t="s">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="5"/>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="3" t="s">
+      <c r="C21" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="5"/>
-      <c r="B19" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="1">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B12"/>
-    <mergeCell ref="A2:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
R2 y R3 complete
</commit_message>
<xml_diff>
--- a/CarDealer/docs/traceabillity.xlsx
+++ b/CarDealer/docs/traceabillity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo Ramos\Desktop\Lab3\CarDealer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E738054C-CA6B-4042-9F03-DEE535682D9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF877B5-9842-4E13-A2A0-BE1E7AD13477}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4344" yWindow="-60" windowWidth="17280" windowHeight="8964" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
+    <workbookView xWindow="1620" yWindow="1560" windowWidth="17280" windowHeight="8964" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>Requirements</t>
   </si>
@@ -130,6 +130,42 @@
   </si>
   <si>
     <t>lookForSpaceinParkingLot(column : int) : int</t>
+  </si>
+  <si>
+    <t>R2. Register the information of a client</t>
+  </si>
+  <si>
+    <t>registerClient():void</t>
+  </si>
+  <si>
+    <t>registerClient(name : String, lastName : String, id : int, phoneNumber : String, email : String) : String</t>
+  </si>
+  <si>
+    <t>searchClient(id : int) : model.Client</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Client(name : String, lastName : String, id : int, phoneNumber : String, email : String)</t>
+  </si>
+  <si>
+    <t>R3. Register the information of a seller</t>
+  </si>
+  <si>
+    <t>registerSeller() : void</t>
+  </si>
+  <si>
+    <t>registerSeller(name : String, lastName : String, id : int) : String</t>
+  </si>
+  <si>
+    <t>searchSeller(id : int) : model.Seller</t>
+  </si>
+  <si>
+    <t>Seller</t>
+  </si>
+  <si>
+    <t>Seller(name : String, lastName : String, id : int)</t>
   </si>
 </sst>
 </file>
@@ -183,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -207,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -522,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE54D6B-CD4A-424B-9A43-965713A2DE34}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="69" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="69" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +589,7 @@
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -559,7 +598,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
-      <c r="B3" s="7"/>
+      <c r="B3" s="10"/>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
@@ -698,11 +737,76 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
todo lo anterior estaba mal, de aqui pa delante todo bien
</commit_message>
<xml_diff>
--- a/CarDealer/docs/traceabillity.xlsx
+++ b/CarDealer/docs/traceabillity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo Ramos\Desktop\Lab3\CarDealer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73A213B9-24F3-40A5-BDB1-66F627714EA9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF95965-5CCB-4912-8B59-E7961E880305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5052" yWindow="3852" windowWidth="17280" windowHeight="8964" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
   <si>
     <t>Requirements</t>
   </si>
@@ -63,18 +63,9 @@
     <t>Business</t>
   </si>
   <si>
-    <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, isNew : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, type : int, gasolineCapacity : double, gasolineConsume : double) : String</t>
-  </si>
-  <si>
     <t>searchVehicle(licensePlate : String) : boolean</t>
   </si>
   <si>
-    <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double) : String</t>
-  </si>
-  <si>
-    <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double, typeCharger : int, batteryDuration : double, batteryConsume : double) : String</t>
-  </si>
-  <si>
     <t>createSoat(price : double, year : int, moneyCovered : double) : model.Soat</t>
   </si>
   <si>
@@ -96,9 +87,6 @@
     <t>Motorcycle</t>
   </si>
   <si>
-    <t>Motorcycle(price : double, brand : String, model : int, displacement : double, milleage : double, isNew : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, type : int, gasolineCapacity : double, gasolineConsume : double)</t>
-  </si>
-  <si>
     <t>GasolineCar</t>
   </si>
   <si>
@@ -108,24 +96,12 @@
     <t>HybridCar</t>
   </si>
   <si>
-    <t>GasolineCar(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double)</t>
-  </si>
-  <si>
-    <t>HybridCar(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, gasolineConsume : double, typeCharger : int, batteryDuration : double, batteryConsume : double)</t>
-  </si>
-  <si>
     <t>Vehicle</t>
   </si>
   <si>
     <t>getLicensePlate() : String</t>
   </si>
   <si>
-    <t>ElectricCar(price : double, brand : String, model : int,displacement:double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double, batteryConsume : double)</t>
-  </si>
-  <si>
-    <t>registerVehicle(price : double, brand : String, model : int, displacement:double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double, batteryConsume : double) : String</t>
-  </si>
-  <si>
     <t>saveInParkingLot(model : int, isNew : boolean) : boolean</t>
   </si>
   <si>
@@ -199,6 +175,36 @@
   </si>
   <si>
     <t>addInterestingVehicle(vehicle : model.Vehicle) : void</t>
+  </si>
+  <si>
+    <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, isNew : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, type : int, gasolineCapacity : double) : String</t>
+  </si>
+  <si>
+    <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int) : String</t>
+  </si>
+  <si>
+    <t>registerVehicle(price : double, brand : String, model : int, displacement:double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double) : String</t>
+  </si>
+  <si>
+    <t>registerVehicle(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int, typeCharger : int, batteryDuration : double) : String</t>
+  </si>
+  <si>
+    <t>Motorcycle(price : double, brand : String, model : int, displacement : double, milleage : double, isNew : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, type : int, gasolineCapacity : double)</t>
+  </si>
+  <si>
+    <t>GasolineCar(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int)</t>
+  </si>
+  <si>
+    <t>ElectricCar(price : double, brand : String, model : int,displacement:double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, typeCharger : int, batteryDuration : double)</t>
+  </si>
+  <si>
+    <t>HybridCar(price : double, brand : String, model : int, displacement : double, milleage : double, new : boolean, licensePlate : String, soat : model.Document, mechanicalTechnicalReview : model.Document, typeOfCar : int, numberOfDoors : int, tintedWindows : boolean, tankCapacity : double, typeOfFuel : int,  typeCharger : int, batteryDuration : double)</t>
+  </si>
+  <si>
+    <t>calculateGasolineConsume() : double</t>
+  </si>
+  <si>
+    <t>decode():String</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -276,6 +282,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -594,10 +606,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE54D6B-CD4A-424B-9A43-965713A2DE34}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="69" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="108" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,7 +634,7 @@
       <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="12" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -631,7 +643,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="9"/>
-      <c r="B3" s="10"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
@@ -656,206 +668,203 @@
       <c r="A6" s="9"/>
       <c r="B6" s="8"/>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="8"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="9"/>
       <c r="B8" s="8"/>
       <c r="C8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="9"/>
       <c r="B9" s="8"/>
       <c r="C9" s="2" t="s">
-        <v>13</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="9"/>
       <c r="B11" s="8"/>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="9"/>
       <c r="B12" s="8"/>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="9"/>
       <c r="B13" s="8"/>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="9"/>
       <c r="B14" s="8"/>
       <c r="C14" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="9"/>
       <c r="B15" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="9"/>
-      <c r="B16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="11"/>
+      <c r="C16" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="9"/>
-      <c r="B17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="9"/>
-      <c r="B18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B18" s="1"/>
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="9"/>
       <c r="B19" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="9"/>
-      <c r="B20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>28</v>
+      <c r="B20" s="10"/>
+      <c r="C20" s="6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C22" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B23" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C24" t="s">
-        <v>36</v>
+      <c r="A22" s="4"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="4"/>
+      <c r="B24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B25" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" t="s">
-        <v>38</v>
+      <c r="A25" s="4"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>39</v>
-      </c>
-      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B27" t="s">
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B28" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C27" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C28" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
         <v>4</v>
       </c>
-      <c r="C30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C31" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -863,62 +872,99 @@
         <v>9</v>
       </c>
       <c r="C32" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B33" t="s">
-        <v>43</v>
-      </c>
       <c r="C33" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34" t="s">
+        <v>35</v>
+      </c>
       <c r="C34" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>51</v>
-      </c>
       <c r="B35" t="s">
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
         <v>9</v>
       </c>
-      <c r="C36" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C37" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
       <c r="C38" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B39" t="s">
-        <v>37</v>
+      <c r="A39" t="s">
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>4</v>
+      </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C43" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>29</v>
+      </c>
+      <c r="C44" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C45" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
todo estaba mal, again. R5 :)
</commit_message>
<xml_diff>
--- a/CarDealer/docs/traceabillity.xlsx
+++ b/CarDealer/docs/traceabillity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo Ramos\Desktop\Lab3\CarDealer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DF95965-5CCB-4912-8B59-E7961E880305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C5FD3-AB05-4103-B1A3-32CF4BD88281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
+    <workbookView xWindow="-7320" yWindow="5496" windowWidth="17280" windowHeight="8964" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
   <si>
     <t>Requirements</t>
   </si>
@@ -205,6 +205,21 @@
   </si>
   <si>
     <t>decode():String</t>
+  </si>
+  <si>
+    <t>printVehicles() : int</t>
+  </si>
+  <si>
+    <t>lookForVehicles(brand : String) : ArrayList&lt;model.Vehicle&gt;</t>
+  </si>
+  <si>
+    <t>lookForVehicles(model : int) : ArrayList&lt;model.Vehicle&gt;</t>
+  </si>
+  <si>
+    <t>lookForVehicles(displacement : double) : ArrayList&lt;model.Vehicle&gt;</t>
+  </si>
+  <si>
+    <t>toString():String</t>
   </si>
 </sst>
 </file>
@@ -606,10 +621,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE54D6B-CD4A-424B-9A43-965713A2DE34}">
-  <dimension ref="A1:C45"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="108" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -921,14 +936,14 @@
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>43</v>
-      </c>
       <c r="C39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
       <c r="B40" t="s">
         <v>4</v>
       </c>
@@ -937,34 +952,62 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B41" t="s">
+      <c r="C41" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
         <v>9</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C42" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C44" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>29</v>
-      </c>
-      <c r="C44" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C50" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
R6 Todo bien por ahora
</commit_message>
<xml_diff>
--- a/CarDealer/docs/traceabillity.xlsx
+++ b/CarDealer/docs/traceabillity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Pablo Ramos\Desktop\Lab3\CarDealer\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091C5FD3-AB05-4103-B1A3-32CF4BD88281}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FC98F9-C0AA-4999-83CF-138DA0E7ACB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7320" yWindow="5496" windowWidth="17280" windowHeight="8964" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{33BF50A6-F299-47D4-BDE9-EA9EF7C18228}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>Requirements</t>
   </si>
@@ -220,6 +220,18 @@
   </si>
   <si>
     <t>toString():String</t>
+  </si>
+  <si>
+    <t>getInterestingVehicles() : ArrayList&lt;model.Vehicle&gt;</t>
+  </si>
+  <si>
+    <t>lookForVehicle(array : ArrayList&lt;model.Vehicle&gt;, vehicle : model.Vehicle) : boolean</t>
+  </si>
+  <si>
+    <t>R6. Show a complete report with all the data of the vehicles of interest of a client</t>
+  </si>
+  <si>
+    <t>showVehiclesOfInterest() : void</t>
   </si>
 </sst>
 </file>
@@ -621,10 +633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DE54D6B-CD4A-424B-9A43-965713A2DE34}">
-  <dimension ref="A1:C50"/>
+  <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -990,24 +1002,66 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B48" t="s">
+      <c r="C48" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
         <v>29</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C49" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
         <v>21</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C52" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>65</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4</v>
+      </c>
+      <c r="C53" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>29</v>
+      </c>
+      <c r="C56" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>